<commit_message>
[R] Clarke Error Grid Analysis
</commit_message>
<xml_diff>
--- a/Data_Result/Test_Mul_GA_compare.xlsx
+++ b/Data_Result/Test_Mul_GA_compare.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Val_BG_compare_with_naive_6" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -657,7 +658,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -692,7 +693,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -879,8 +880,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X58" sqref="X58"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="Q49" sqref="Q49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>

</xml_diff>